<commit_message>
add: add data desc code
</commit_message>
<xml_diff>
--- a/data/ALL_data_grouped_processed_des.xlsx
+++ b/data/ALL_data_grouped_processed_des.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG9"/>
+  <dimension ref="A1:BI9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,861 +434,892 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Dmax(mm)</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Tg(K)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Tx(K)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Tl(K)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>yield(MPa)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Modulus (GPa)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Ε(%)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Ni</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Nb</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Fe</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Mo</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Co</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Au</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Ge</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Pd</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Cu</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Zr</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Ti</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Al</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Mg</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Gd</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>La</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Ga</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Hf</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Sn</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>In</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Ca</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Zn</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Nd</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Er</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Dy</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Pr</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Ho</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Ce</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Sc</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Ta</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Mn</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Tm</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Pt</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Tb</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Li</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Sm</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Lu</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Yb</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>Pb</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>Sr</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Ru</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Be</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>cls_label</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>805</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>871</v>
+        <v>812</v>
       </c>
       <c r="C2" t="n">
-        <v>812</v>
+        <v>878</v>
       </c>
       <c r="D2" t="n">
-        <v>811</v>
+        <v>820</v>
       </c>
       <c r="E2" t="n">
-        <v>320</v>
+        <v>815</v>
       </c>
       <c r="F2" t="n">
-        <v>391</v>
+        <v>326</v>
       </c>
       <c r="G2" t="n">
-        <v>280</v>
+        <v>399</v>
       </c>
       <c r="H2" t="n">
-        <v>1269</v>
+        <v>288</v>
       </c>
       <c r="I2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="J2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="K2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="L2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="M2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="N2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="O2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="P2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="Q2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="R2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="S2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="T2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="U2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="V2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="W2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="X2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="Y2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="Z2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AA2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AB2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AC2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AD2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AE2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AF2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AG2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AH2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AI2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AK2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AL2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AM2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AN2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AO2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AP2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AR2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AS2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AT2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AU2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AV2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AW2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AX2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AY2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BA2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BB2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BC2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BD2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BE2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BF2" t="n">
-        <v>1269</v>
+        <v>1276</v>
       </c>
       <c r="BG2" t="n">
-        <v>1269</v>
+        <v>1276</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>1276</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>1276</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>5.472894409937888</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>625.4120283199388</v>
+        <v>5.44295566502463</v>
       </c>
       <c r="C3" t="n">
-        <v>676.4246408045977</v>
+        <v>625.9098823082765</v>
       </c>
       <c r="D3" t="n">
-        <v>1075.919340320592</v>
+        <v>677.0424491869919</v>
       </c>
       <c r="E3" t="n">
-        <v>1542.71484375</v>
+        <v>1076.76145398773</v>
       </c>
       <c r="F3" t="n">
-        <v>94.93711338448422</v>
+        <v>1547.051380368098</v>
       </c>
       <c r="G3" t="n">
-        <v>10.80166369047619</v>
+        <v>94.64789807852965</v>
       </c>
       <c r="H3" t="n">
-        <v>7.705899159364328</v>
+        <v>10.65647858796296</v>
       </c>
       <c r="I3" t="n">
-        <v>1.757968630260047</v>
+        <v>7.663625417894462</v>
       </c>
       <c r="J3" t="n">
-        <v>2.531229395744681</v>
+        <v>1.748324601724138</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8972608353033883</v>
+        <v>2.517343341065831</v>
       </c>
       <c r="L3" t="n">
-        <v>1.969253821907014</v>
+        <v>0.8923385579937303</v>
       </c>
       <c r="M3" t="n">
-        <v>0.7897307342789599</v>
+        <v>1.958450705329154</v>
       </c>
       <c r="N3" t="n">
-        <v>10.15173316469661</v>
+        <v>0.7853983556426333</v>
       </c>
       <c r="O3" t="n">
-        <v>0.7276483769897557</v>
+        <v>10.09604183855799</v>
       </c>
       <c r="P3" t="n">
-        <v>1.721290255476753</v>
+        <v>0.7236565755485893</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8200179100866825</v>
+        <v>1.711847440595611</v>
       </c>
       <c r="R3" t="n">
-        <v>3.374662150985028</v>
+        <v>0.8155193792319749</v>
       </c>
       <c r="S3" t="n">
-        <v>0.4095350669818755</v>
+        <v>3.356149114106584</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03393223010244287</v>
+        <v>0.4072884012539185</v>
       </c>
       <c r="U3" t="n">
-        <v>2.067297084318361</v>
+        <v>0.03374608150470219</v>
       </c>
       <c r="V3" t="n">
-        <v>14.30319076246388</v>
+        <v>2.055956112852665</v>
       </c>
       <c r="W3" t="n">
-        <v>15.55751966485421</v>
+        <v>14.37032843069488</v>
       </c>
       <c r="X3" t="n">
-        <v>4.066851112923562</v>
+        <v>15.61777621841693</v>
       </c>
       <c r="Y3" t="n">
-        <v>6.022582594562648</v>
+        <v>4.044540801175549</v>
       </c>
       <c r="Z3" t="n">
-        <v>5.882695035460993</v>
+        <v>5.989543348354232</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.589913317572892</v>
+        <v>5.850423197492163</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.7491725768321513</v>
+        <v>1.581191222570533</v>
       </c>
       <c r="AC3" t="n">
-        <v>3.545784081954295</v>
+        <v>0.7450626959247649</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.0425531914893617</v>
+        <v>3.526332288401254</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.124142927265563</v>
+        <v>0.04231974921630094</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.1245547675334909</v>
+        <v>1.117975998981191</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.007092198581560284</v>
+        <v>0.123871473354232</v>
       </c>
       <c r="AH3" t="n">
-        <v>3.776674546887313</v>
+        <v>0.007053291536050157</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.6028368794326241</v>
+        <v>3.755956112852664</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.3685579196217494</v>
+        <v>0.5995297805642633</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.1601457840819543</v>
+        <v>0.3665360501567398</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.1599684791174153</v>
+        <v>0.1592672413793103</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.975177304964539</v>
+        <v>0.1590909090909091</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.1646966115051221</v>
+        <v>0.9698275862068966</v>
       </c>
       <c r="AO3" t="n">
-        <v>2.061229314420804</v>
+        <v>0.1637931034482759</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.1379038613081166</v>
+        <v>2.049921630094044</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.8490640630417653</v>
+        <v>0.1371473354231975</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1533718088258472</v>
+        <v>0.8444061880877745</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.1952583845547675</v>
+        <v>0.1525304274294671</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.2736012608353034</v>
+        <v>0.1941872178683386</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.007662577462569</v>
+        <v>0.2721003134796238</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.3386190398739165</v>
+        <v>1.002134647962382</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.1007722616233254</v>
+        <v>0.3367614119122257</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.07313632781717887</v>
+        <v>0.1002194357366771</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.07486209613869188</v>
+        <v>0.07273510971786833</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.1095350669818755</v>
+        <v>0.07445141065830721</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.1107171000788022</v>
+        <v>0.1089341692789969</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.001576044129235619</v>
+        <v>0.1101097178683386</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.2442868400315209</v>
+        <v>0.001567398119122257</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.08668242710795902</v>
+        <v>0.2429467084639498</v>
       </c>
       <c r="BE3" t="n">
-        <v>0</v>
+        <v>0.08620689655172414</v>
       </c>
       <c r="BF3" t="n">
         <v>0</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.8384554767533491</v>
+        <v>0</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.2573824451410658</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0.8393416927899686</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>5.430753289239727</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>172.2104111356758</v>
+        <v>5.416799973795269</v>
       </c>
       <c r="C4" t="n">
-        <v>176.7289916310277</v>
+        <v>171.6169442003815</v>
       </c>
       <c r="D4" t="n">
-        <v>265.9006960655317</v>
+        <v>175.9817916165378</v>
       </c>
       <c r="E4" t="n">
-        <v>502.9354187947058</v>
+        <v>265.5534544707519</v>
       </c>
       <c r="F4" t="n">
-        <v>52.99942205420455</v>
+        <v>500.5836485157467</v>
       </c>
       <c r="G4" t="n">
-        <v>12.93810686313891</v>
+        <v>52.51453634171216</v>
       </c>
       <c r="H4" t="n">
-        <v>14.43346693300463</v>
+        <v>12.80005776396969</v>
       </c>
       <c r="I4" t="n">
-        <v>5.287464501756245</v>
+        <v>14.40504935775119</v>
       </c>
       <c r="J4" t="n">
-        <v>6.754250447766057</v>
+        <v>5.274529743985168</v>
       </c>
       <c r="K4" t="n">
-        <v>3.697799905897613</v>
+        <v>6.738280218547899</v>
       </c>
       <c r="L4" t="n">
-        <v>5.699529242158444</v>
+        <v>3.688231080096602</v>
       </c>
       <c r="M4" t="n">
-        <v>2.840631030449611</v>
+        <v>5.685724275729099</v>
       </c>
       <c r="N4" t="n">
-        <v>21.58336133597282</v>
+        <v>2.833423469413276</v>
       </c>
       <c r="O4" t="n">
-        <v>2.984730810999582</v>
+        <v>21.53709888552774</v>
       </c>
       <c r="P4" t="n">
-        <v>5.243466376815008</v>
+        <v>2.977011742242182</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.792461522792772</v>
+        <v>5.230599378830392</v>
       </c>
       <c r="R4" t="n">
-        <v>8.241942753428267</v>
+        <v>3.782521873248275</v>
       </c>
       <c r="S4" t="n">
-        <v>5.093805744266557</v>
+        <v>8.223068445491055</v>
       </c>
       <c r="T4" t="n">
-        <v>0.6672454311834325</v>
+        <v>5.07989363929634</v>
       </c>
       <c r="U4" t="n">
-        <v>11.1812580071403</v>
+        <v>0.665415980011918</v>
       </c>
       <c r="V4" t="n">
-        <v>16.48406269562467</v>
+        <v>11.1515684198406</v>
       </c>
       <c r="W4" t="n">
-        <v>22.78300302513043</v>
+        <v>16.47295419333211</v>
       </c>
       <c r="X4" t="n">
-        <v>9.169522313735968</v>
+        <v>22.74163871411715</v>
       </c>
       <c r="Y4" t="n">
-        <v>7.929484486384768</v>
+        <v>9.149252906594466</v>
       </c>
       <c r="Z4" t="n">
-        <v>16.57990182793011</v>
+        <v>7.92019973739828</v>
       </c>
       <c r="AA4" t="n">
-        <v>6.414745206556176</v>
+        <v>16.54003867438572</v>
       </c>
       <c r="AB4" t="n">
-        <v>5.041524075995004</v>
+        <v>6.398190552381331</v>
       </c>
       <c r="AC4" t="n">
-        <v>13.90404858274012</v>
+        <v>5.027970306975853</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.427930726118295</v>
+        <v>13.8683032660278</v>
       </c>
       <c r="AE4" t="n">
-        <v>5.253643912111099</v>
+        <v>0.4267659812804789</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.8341415776027074</v>
+        <v>5.239860740265721</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.2043227062922713</v>
+        <v>0.8318995390525159</v>
       </c>
       <c r="AH4" t="n">
-        <v>13.38679694571346</v>
+        <v>0.2037617223884945</v>
       </c>
       <c r="AI4" t="n">
-        <v>3.430624947347697</v>
+        <v>13.35291478009004</v>
       </c>
       <c r="AJ4" t="n">
-        <v>4.255408088259983</v>
+        <v>3.421484566889841</v>
       </c>
       <c r="AK4" t="n">
-        <v>2.359522955787455</v>
+        <v>4.243797881877596</v>
       </c>
       <c r="AL4" t="n">
-        <v>2.368718057430793</v>
+        <v>2.3530666748669</v>
       </c>
       <c r="AM4" t="n">
-        <v>7.678756598970652</v>
+        <v>2.362236319212684</v>
       </c>
       <c r="AN4" t="n">
-        <v>2.564096068792352</v>
+        <v>7.657987672093526</v>
       </c>
       <c r="AO4" t="n">
-        <v>11.1229071501933</v>
+        <v>2.557076646021944</v>
       </c>
       <c r="AP4" t="n">
-        <v>2.143669946454095</v>
+        <v>11.09337728564644</v>
       </c>
       <c r="AQ4" t="n">
-        <v>4.041652497877916</v>
+        <v>2.137801549200824</v>
       </c>
       <c r="AR4" t="n">
-        <v>1.509991139991273</v>
+        <v>4.031030765380454</v>
       </c>
       <c r="AS4" t="n">
-        <v>2.87484621307196</v>
+        <v>1.505883006941647</v>
       </c>
       <c r="AT4" t="n">
-        <v>3.971889160505648</v>
+        <v>2.866979921727244</v>
       </c>
       <c r="AU4" t="n">
-        <v>4.495458317642224</v>
+        <v>3.961022523081721</v>
       </c>
       <c r="AV4" t="n">
-        <v>3.098775666522295</v>
+        <v>4.483719146973247</v>
       </c>
       <c r="AW4" t="n">
-        <v>1.891608824712022</v>
+        <v>3.090358811255201</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.9384063935607956</v>
+        <v>1.886423722712931</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.908367780967391</v>
+        <v>0.9358424345621036</v>
       </c>
       <c r="AZ4" t="n">
-        <v>2.273800620802554</v>
+        <v>1.903129953624377</v>
       </c>
       <c r="BA4" t="n">
-        <v>2.066461613986859</v>
+        <v>2.26756466937121</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.05614346140443459</v>
+        <v>2.060797406038949</v>
       </c>
       <c r="BC4" t="n">
-        <v>3.510267845432879</v>
+        <v>0.05598925109558543</v>
       </c>
       <c r="BD4" t="n">
-        <v>1.781535361340085</v>
+        <v>3.500665093151969</v>
       </c>
       <c r="BE4" t="n">
-        <v>0</v>
+        <v>1.776649687160002</v>
       </c>
       <c r="BF4" t="n">
         <v>0</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.3681775527627784</v>
+        <v>0</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>3.640204848509379</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.367359467084253</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0.06</v>
-      </c>
-      <c r="B5" t="n">
-        <v>293</v>
       </c>
       <c r="C5" t="n">
         <v>293</v>
       </c>
       <c r="D5" t="n">
+        <v>293</v>
+      </c>
+      <c r="E5" t="n">
         <v>581</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>140.5</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>16</v>
       </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
@@ -1443,33 +1474,41 @@
         <v>0</v>
       </c>
       <c r="BG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>2</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>426</v>
       </c>
-      <c r="C6" t="n">
-        <v>477</v>
-      </c>
       <c r="D6" t="n">
-        <v>792.2</v>
+        <v>477.75</v>
       </c>
       <c r="E6" t="n">
-        <v>1304.75</v>
+        <v>794.5</v>
       </c>
       <c r="F6" t="n">
-        <v>61.18</v>
+        <v>1306.75</v>
       </c>
       <c r="G6" t="n">
-        <v>1.7</v>
+        <v>61.745</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1.7925</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1622,33 +1661,41 @@
         <v>0</v>
       </c>
       <c r="BG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>4</v>
       </c>
-      <c r="B7" t="n">
-        <v>668.4</v>
-      </c>
       <c r="C7" t="n">
+        <v>668.95</v>
+      </c>
+      <c r="D7" t="n">
         <v>732</v>
       </c>
-      <c r="D7" t="n">
-        <v>1145</v>
-      </c>
       <c r="E7" t="n">
-        <v>1581.5</v>
+        <v>1147</v>
       </c>
       <c r="F7" t="n">
-        <v>88.7</v>
+        <v>1589</v>
       </c>
       <c r="G7" t="n">
-        <v>5.6</v>
+        <v>88</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>5.57</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1690,10 +1737,10 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>9.4</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1801,37 +1848,45 @@
         <v>0</v>
       </c>
       <c r="BG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>740</v>
       </c>
-      <c r="C8" t="n">
-        <v>796.8499999999999</v>
-      </c>
       <c r="D8" t="n">
+        <v>796</v>
+      </c>
+      <c r="E8" t="n">
         <v>1267.5</v>
       </c>
-      <c r="E8" t="n">
-        <v>1797.625</v>
-      </c>
       <c r="F8" t="n">
-        <v>108.4</v>
+        <v>1799.5</v>
       </c>
       <c r="G8" t="n">
-        <v>14.625</v>
+        <v>106.4</v>
       </c>
       <c r="H8" t="n">
+        <v>13.475</v>
+      </c>
+      <c r="I8" t="n">
         <v>10</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
@@ -1845,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>2.125</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -1869,20 +1924,20 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>24.75</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
+        <v>24.925</v>
+      </c>
+      <c r="X8" t="n">
         <v>30</v>
       </c>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
       <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
         <v>10</v>
       </c>
-      <c r="Z8" t="n">
-        <v>0</v>
-      </c>
       <c r="AA8" t="n">
         <v>0</v>
       </c>
@@ -1980,185 +2035,199 @@
         <v>0</v>
       </c>
       <c r="BG8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>35</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>1135</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>1019</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>1725</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>4014</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>309</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>75</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>100</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>27.2727273</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>50</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>25</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>35</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>25</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>91</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>23.0769231</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>52</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>56</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>64.80000000000001</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>77.8</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>13.8</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>95</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
         <v>64</v>
       </c>
-      <c r="W9" t="n">
+      <c r="X9" t="n">
         <v>72</v>
       </c>
-      <c r="X9" t="n">
+      <c r="Y9" t="n">
         <v>53</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="Z9" t="n">
         <v>88</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AA9" t="n">
         <v>90</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AB9" t="n">
         <v>61.5</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AC9" t="n">
         <v>60</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AD9" t="n">
         <v>70</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AE9" t="n">
         <v>7.5</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AF9" t="n">
         <v>51</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AG9" t="n">
         <v>20</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AH9" t="n">
         <v>7</v>
       </c>
-      <c r="AH9" t="n">
+      <c r="AI9" t="n">
         <v>70</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AJ9" t="n">
         <v>40</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AK9" t="n">
         <v>67.5</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>55</v>
       </c>
       <c r="AL9" t="n">
         <v>55</v>
       </c>
       <c r="AM9" t="n">
+        <v>55</v>
+      </c>
+      <c r="AN9" t="n">
         <v>72</v>
       </c>
-      <c r="AN9" t="n">
+      <c r="AO9" t="n">
         <v>55</v>
       </c>
-      <c r="AO9" t="n">
+      <c r="AP9" t="n">
         <v>70</v>
       </c>
-      <c r="AP9" t="n">
+      <c r="AQ9" t="n">
         <v>46</v>
       </c>
-      <c r="AQ9" t="n">
+      <c r="AR9" t="n">
         <v>42</v>
       </c>
-      <c r="AR9" t="n">
+      <c r="AS9" t="n">
         <v>19.2</v>
       </c>
-      <c r="AS9" t="n">
+      <c r="AT9" t="n">
         <v>55</v>
       </c>
-      <c r="AT9" t="n">
+      <c r="AU9" t="n">
         <v>74.7</v>
       </c>
-      <c r="AU9" t="n">
+      <c r="AV9" t="n">
         <v>42.8571429</v>
       </c>
-      <c r="AV9" t="n">
+      <c r="AW9" t="n">
         <v>46</v>
       </c>
-      <c r="AW9" t="n">
+      <c r="AX9" t="n">
         <v>55</v>
       </c>
-      <c r="AX9" t="n">
+      <c r="AY9" t="n">
         <v>20</v>
-      </c>
-      <c r="AY9" t="n">
-        <v>55</v>
       </c>
       <c r="AZ9" t="n">
         <v>55</v>
       </c>
       <c r="BA9" t="n">
+        <v>55</v>
+      </c>
+      <c r="BB9" t="n">
         <v>62.5</v>
       </c>
-      <c r="BB9" t="n">
+      <c r="BC9" t="n">
         <v>2</v>
       </c>
-      <c r="BC9" t="n">
+      <c r="BD9" t="n">
         <v>60</v>
       </c>
-      <c r="BD9" t="n">
+      <c r="BE9" t="n">
         <v>37</v>
       </c>
-      <c r="BE9" t="n">
-        <v>0</v>
-      </c>
       <c r="BF9" t="n">
         <v>0</v>
       </c>
       <c r="BG9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="BI9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>